<commit_message>
fix xong danh muc phan cap cha con
</commit_message>
<xml_diff>
--- a/Assets/Excel/Category/Category.xlsx
+++ b/Assets/Excel/Category/Category.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teu-laptop\source\repos\QuanLyHoSo\Assets\Excel\Category\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8AC5EB-8708-4F3B-A23F-9CDEF3E063C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC652AEE-CE38-4D01-B812-474D8DB8972B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{5D827FDB-3D87-44DC-BC1E-84EB5B696D4D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D827FDB-3D87-44DC-BC1E-84EB5B696D4D}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>TrangThai</t>
   </si>
@@ -43,9 +43,6 @@
     <t>MoTa</t>
   </si>
   <si>
-    <t>kho excel test thu</t>
-  </si>
-  <si>
     <t>TenDanhMuc</t>
   </si>
   <si>
@@ -55,94 +52,121 @@
     <t>MaDanhMucCha</t>
   </si>
   <si>
-    <t>danhmuc ex1</t>
-  </si>
-  <si>
-    <t>danhmuc ex2</t>
-  </si>
-  <si>
-    <t>danhmuc ex3</t>
-  </si>
-  <si>
-    <t>danhmuc ex4</t>
-  </si>
-  <si>
-    <t>danhmuc ex5</t>
-  </si>
-  <si>
-    <t>danhmuc ex6</t>
-  </si>
-  <si>
-    <t>danhmuc ex7</t>
-  </si>
-  <si>
-    <t>danhmuc ex8</t>
-  </si>
-  <si>
-    <t>danhmuc ex9</t>
-  </si>
-  <si>
-    <t>danhmuc ex10</t>
-  </si>
-  <si>
-    <t>danhmuc ex11</t>
-  </si>
-  <si>
-    <t>danhmuc ex12</t>
-  </si>
-  <si>
-    <t>danhmuc ex13</t>
-  </si>
-  <si>
-    <t>danhmuc ex14</t>
-  </si>
-  <si>
-    <t>danhmuc ex15</t>
-  </si>
-  <si>
-    <t>dme2</t>
-  </si>
-  <si>
-    <t>dme3</t>
-  </si>
-  <si>
-    <t>dme4</t>
-  </si>
-  <si>
-    <t>dme5</t>
-  </si>
-  <si>
-    <t>dme6</t>
-  </si>
-  <si>
-    <t>dme7</t>
-  </si>
-  <si>
-    <t>dme8</t>
-  </si>
-  <si>
-    <t>dme9</t>
-  </si>
-  <si>
-    <t>dme10</t>
-  </si>
-  <si>
-    <t>dme11</t>
-  </si>
-  <si>
-    <t>dme12</t>
-  </si>
-  <si>
-    <t>dme13</t>
-  </si>
-  <si>
-    <t>dme14</t>
-  </si>
-  <si>
-    <t>dme15</t>
-  </si>
-  <si>
-    <t>parrent</t>
+    <t>danhmuc3</t>
+  </si>
+  <si>
+    <t>dm3</t>
+  </si>
+  <si>
+    <t>danhmuc4</t>
+  </si>
+  <si>
+    <t>dm4</t>
+  </si>
+  <si>
+    <t>danhmuc5</t>
+  </si>
+  <si>
+    <t>dm5</t>
+  </si>
+  <si>
+    <t>danhmuc6</t>
+  </si>
+  <si>
+    <t>dm6</t>
+  </si>
+  <si>
+    <t>danhmuc7</t>
+  </si>
+  <si>
+    <t>dm7</t>
+  </si>
+  <si>
+    <t>danhmuc8</t>
+  </si>
+  <si>
+    <t>dm8</t>
+  </si>
+  <si>
+    <t>danhmuc9</t>
+  </si>
+  <si>
+    <t>dm9</t>
+  </si>
+  <si>
+    <t>danhmuc10</t>
+  </si>
+  <si>
+    <t>dm10</t>
+  </si>
+  <si>
+    <t>danhmuc11</t>
+  </si>
+  <si>
+    <t>dm11</t>
+  </si>
+  <si>
+    <t>danhmuc12</t>
+  </si>
+  <si>
+    <t>dm12</t>
+  </si>
+  <si>
+    <t>danhmuc13</t>
+  </si>
+  <si>
+    <t>dm13</t>
+  </si>
+  <si>
+    <t>danhmuc14</t>
+  </si>
+  <si>
+    <t>dm14</t>
+  </si>
+  <si>
+    <t>danhmuc15</t>
+  </si>
+  <si>
+    <t>dm15</t>
+  </si>
+  <si>
+    <t>danhmuc16</t>
+  </si>
+  <si>
+    <t>dm16</t>
+  </si>
+  <si>
+    <t>danhmuc17</t>
+  </si>
+  <si>
+    <t>dm17</t>
+  </si>
+  <si>
+    <t>danhmuc18</t>
+  </si>
+  <si>
+    <t>dm18</t>
+  </si>
+  <si>
+    <t>danhmuc19</t>
+  </si>
+  <si>
+    <t>dm19</t>
+  </si>
+  <si>
+    <t>danhmuc20</t>
+  </si>
+  <si>
+    <t>dm20</t>
+  </si>
+  <si>
+    <t>danhmuc21</t>
+  </si>
+  <si>
+    <t>dm21</t>
+  </si>
+  <si>
+    <t>dm2</t>
   </si>
 </sst>
 </file>
@@ -514,30 +538,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C34D6A-8752-4C76-BC59-E44550E99B6D}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -548,7 +572,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -556,219 +592,305 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>2</v>
+      <c r="E6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>2</v>
+      <c r="E8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>2</v>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>2</v>
+      <c r="E12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>2</v>
+      <c r="E14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
       </c>
       <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
list danh muc phan cap
</commit_message>
<xml_diff>
--- a/Assets/Excel/Category/Category.xlsx
+++ b/Assets/Excel/Category/Category.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teu-pc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D84D56-3D95-44C4-A63C-C016A8F7E88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744AF0B6-8B9C-410B-B5DD-42D1D645B1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>TenDanhMuc</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Đóng</t>
   </si>
   <si>
-    <t>danh mục 1</t>
+    <t>danh muc 1</t>
   </si>
   <si>
     <t>dm1</t>
@@ -62,44 +62,37 @@
     <t>Mở</t>
   </si>
   <si>
-    <t>excel 1</t>
-  </si>
-  <si>
-    <t>excel 2</t>
-  </si>
-  <si>
-    <t>excel 3</t>
-  </si>
-  <si>
-    <t>excel 4</t>
-  </si>
-  <si>
-    <t>danh muc excel 1</t>
-  </si>
-  <si>
-    <t>danh muc excel 2</t>
-  </si>
-  <si>
-    <t>danh muc excel 3</t>
-  </si>
-  <si>
-    <t>danh muc excel 4</t>
-  </si>
-  <si>
-    <t>danh muc excel 5</t>
+    <t>danh muc 2</t>
+  </si>
+  <si>
+    <t>dm2</t>
+  </si>
+  <si>
+    <t>danh muc 3</t>
+  </si>
+  <si>
+    <t>dm3</t>
+  </si>
+  <si>
+    <t>danh muc 4</t>
+  </si>
+  <si>
+    <t>dm4</t>
+  </si>
+  <si>
+    <t>danh muc goc</t>
+  </si>
+  <si>
+    <t>dmgoc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -144,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E7">
-  <autoFilter ref="A1:E7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E2">
+  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TenDanhMuc"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MaDanhMuc"/>
@@ -158,8 +151,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:B3">
-  <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:B6">
+  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TenDanhMucCha"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="MaDanhMuc"/>
@@ -476,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -510,64 +503,22 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -575,17 +526,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" xr:uid="{F902B968-056E-4112-93F6-FE966F93EA4D}">
+        <x14:dataValidation type="list" xr:uid="{E2ED4468-1409-45E5-AB71-E85754B27417}">
           <x14:formula1>
-            <xm:f>ThongTinBang!$B$2:$B$3</xm:f>
+            <xm:f>ThongTinBang!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C7</xm:sqref>
+          <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" xr:uid="{ADA78EBC-4E50-42AE-B300-DBB5C246F929}">
+        <x14:dataValidation type="list" xr:uid="{E6692AC2-B75A-48A3-A04A-39861F1D5A89}">
           <x14:formula1>
             <xm:f>ThongTinBang!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D7</xm:sqref>
+          <xm:sqref>D2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -595,9 +546,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -649,6 +602,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>